<commit_message>
FIX: Log return to arithmetic return
</commit_message>
<xml_diff>
--- a/lifelib/libraries/appliedlife/economic_data/index_parameters.xlsx
+++ b/lifelib/libraries/appliedlife/economic_data/index_parameters.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27630"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27809"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7e058ec69bd94c7d/pyproj/lifelib/lifelib/libraries/appliedlife/financial_data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fumito\OneDrive\pyproj\lifelib\lifelib\libraries\appliedlife\economic_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="8_{90A6C9E2-FD7D-4F5B-899F-3D42D493DF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CE85613E-3894-48CE-910E-C33324936D6A}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF300578-98BA-4558-BC23-70EB9F389748}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18000" xr2:uid="{F5B2B069-9A58-4E80-81E2-C1C5DAF20EF5}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>FUND1</t>
   </si>
@@ -75,6 +75,12 @@
   </si>
   <si>
     <t>FUND6</t>
+  </si>
+  <si>
+    <t>sharpe_ratio</t>
+  </si>
+  <si>
+    <t>risk_free</t>
   </si>
 </sst>
 </file>
@@ -459,13 +465,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC57DCA-DFDC-4EA8-9D66-1F17A436977D}">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.69140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
@@ -524,10 +533,10 @@
         <v>0.02</v>
       </c>
       <c r="E3" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F3" s="1">
         <v>0.08</v>
-      </c>
-      <c r="F3" s="1">
-        <v>0.09</v>
       </c>
       <c r="G3" s="1">
         <v>0.1</v>
@@ -538,37 +547,75 @@
         <v>6</v>
       </c>
       <c r="B4" s="1">
+        <v>0.08</v>
+      </c>
+      <c r="C4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.12</v>
+      </c>
+      <c r="G4" s="1">
         <v>0.2</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="D4" s="1">
-        <v>0.1</v>
-      </c>
-      <c r="E4" s="1">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="G4" s="1">
-        <v>0.5</v>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.03</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.05</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2">
+        <f t="shared" ref="B6:G6" si="0">(B3-B5)/B4</f>
+        <v>0.25000000000000006</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.24999999999999986</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25</v>
+      </c>
+      <c r="G6" s="2">
+        <f>(G3-G5)/G4</f>
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>